<commit_message>
Redoing all the effects.
</commit_message>
<xml_diff>
--- a/New_game_effects.xlsx
+++ b/New_game_effects.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\barhh\Pycharm projects\Card_Generation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D27A7C8-8D02-4BFA-8ADC-5778F48BA9C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD6A5A18-13D2-49AE-9B07-6B74D7F022F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14280" yWindow="0" windowWidth="8856" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
+    <sheet name="Feuil1" sheetId="2" r:id="rId1"/>
+    <sheet name="Feuil2" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,19 +26,223 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
-  <si>
-    <t>Test</t>
-  </si>
-  <si>
-    <t>allo</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
+  <si>
+    <t>Card Effect #1</t>
+  </si>
+  <si>
+    <t>Card ID</t>
+  </si>
+  <si>
+    <t>Card Effect #2</t>
+  </si>
+  <si>
+    <t>Card Effect #3</t>
+  </si>
+  <si>
+    <t>Trigger</t>
+  </si>
+  <si>
+    <t>Action</t>
+  </si>
+  <si>
+    <t>Action Target</t>
+  </si>
+  <si>
+    <t>Downside</t>
+  </si>
+  <si>
+    <t>SPONTANEOUS</t>
+  </si>
+  <si>
+    <t>Other Keywords</t>
+  </si>
+  <si>
+    <t>RETALIATE</t>
+  </si>
+  <si>
+    <t>MANUAL</t>
+  </si>
+  <si>
+    <t>ONGOING</t>
+  </si>
+  <si>
+    <t>Restriction</t>
+  </si>
+  <si>
+    <t>RESTRICT 1</t>
+  </si>
+  <si>
+    <t>RESTRICT 2</t>
+  </si>
+  <si>
+    <t>RESTRICT 3</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>PLAN PHASE</t>
+  </si>
+  <si>
+    <t>ESCAPE PHASE</t>
+  </si>
+  <si>
+    <t>FINAL PHASE</t>
+  </si>
+  <si>
+    <t>PREPARE PHASE</t>
+  </si>
+  <si>
+    <t>Vanish</t>
+  </si>
+  <si>
+    <t>Disintegrate</t>
+  </si>
+  <si>
+    <t>Draw</t>
+  </si>
+  <si>
+    <t>Mill</t>
+  </si>
+  <si>
+    <t>1 card</t>
+  </si>
+  <si>
+    <t>2 cards</t>
+  </si>
+  <si>
+    <t>3 cards</t>
+  </si>
+  <si>
+    <t>1 anomaly</t>
+  </si>
+  <si>
+    <t>1 room</t>
+  </si>
+  <si>
+    <t>1 activator</t>
+  </si>
+  <si>
+    <t>2 anomalies</t>
+  </si>
+  <si>
+    <t>2 rooms</t>
+  </si>
+  <si>
+    <t>1 &lt;specific card name&gt;</t>
+  </si>
+  <si>
+    <t>1 &lt;specific card name&gt; and 1 &lt;other specific card name&gt;</t>
+  </si>
+  <si>
+    <t>1 &lt;specific card name&gt; or 1 &lt;other specific card name&gt;</t>
+  </si>
+  <si>
+    <t>1 red card</t>
+  </si>
+  <si>
+    <t>1 green card</t>
+  </si>
+  <si>
+    <t>1 orange card</t>
+  </si>
+  <si>
+    <t>1 purple card</t>
+  </si>
+  <si>
+    <t>1 black card</t>
+  </si>
+  <si>
+    <t>1 gray card</t>
+  </si>
+  <si>
+    <t>1 red room</t>
+  </si>
+  <si>
+    <t>1 red anomaly</t>
+  </si>
+  <si>
+    <t>1 red activator</t>
+  </si>
+  <si>
+    <t>1 green anomaly</t>
+  </si>
+  <si>
+    <t>1 green room</t>
+  </si>
+  <si>
+    <t>1 green activator</t>
+  </si>
+  <si>
+    <t>1 orange anomaly</t>
+  </si>
+  <si>
+    <t>1 orange room</t>
+  </si>
+  <si>
+    <t>1 orange activator</t>
+  </si>
+  <si>
+    <t>1 purple anomaly</t>
+  </si>
+  <si>
+    <t>1 purple room</t>
+  </si>
+  <si>
+    <t>1 purple activator</t>
+  </si>
+  <si>
+    <t>1 gray anomaly</t>
+  </si>
+  <si>
+    <t>1 gray room</t>
+  </si>
+  <si>
+    <t>1 gray activator</t>
+  </si>
+  <si>
+    <t>1 black anomaly</t>
+  </si>
+  <si>
+    <t>1 black room</t>
+  </si>
+  <si>
+    <t>1 black activator</t>
+  </si>
+  <si>
+    <t>discard 1 card.</t>
+  </si>
+  <si>
+    <t>exhaust 1 card.</t>
+  </si>
+  <si>
+    <t>exhaust 2 cards.</t>
+  </si>
+  <si>
+    <t>exhaust 1 anomaly.</t>
+  </si>
+  <si>
+    <t>exhaust 1 activator.</t>
+  </si>
+  <si>
+    <t>vanish 1 card you own.</t>
+  </si>
+  <si>
+    <t>disintegrate 1 card you own.</t>
+  </si>
+  <si>
+    <t>DOUBLE AMBUSH</t>
+  </si>
+  <si>
+    <t>IMMUNE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -45,16 +250,34 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -62,12 +285,36 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -347,23 +594,328 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{530D00D6-A3A9-494A-B58E-0CE32A85C62B}">
+  <dimension ref="A1:G36"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="47.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="11.5546875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E7" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E10" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E11" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E12" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E13" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E14" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E15" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E16" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E17" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E18" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E19" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="20" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E20" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="21" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E21" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="22" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E22" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="23" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E23" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="24" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E24" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="25" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E25" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="26" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E26" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="27" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E27" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="28" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E28" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="29" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E29" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="30" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E30" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="31" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E31" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="32" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E32" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="33" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E33" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="34" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E34" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="35" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E35" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="36" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E36" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="7" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="12.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.88671875" style="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B2" t="s">
-        <v>1</v>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>